<commit_message>
Fixes #15: Add configuration for jexunit.dateTimePattern
</commit_message>
<xml_diff>
--- a/examples-simple/src/test/resources/FormattingTest.xlsx
+++ b/examples-simple/src/test/resources/FormattingTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricvog01\IdeaProjects\jexunit\examples-simple\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871CEACD-4810-4C65-914B-E8513C2A6ACD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76EC038-6B7A-4E8F-B146-A7A109B6A48F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="48" windowWidth="21312" windowHeight="10032" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="48" windowWidth="21312" windowHeight="10032" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Empty formatted cell" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>disabled</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>integer</t>
+  </si>
+  <si>
+    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -112,11 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -513,18 +517,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFD8D41-9D87-41AD-8809-B5594C3DBE8E}">
-  <dimension ref="A3:B6"/>
+  <dimension ref="A3:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -532,21 +537,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3">
         <f ca="1">TODAY()</f>
-        <v>43935</v>
+        <v>43938</v>
+      </c>
+      <c r="C6" s="4">
+        <f ca="1">NOW()</f>
+        <v>43938.578615856481</v>
       </c>
     </row>
   </sheetData>
@@ -590,11 +602,11 @@
       </c>
       <c r="B6">
         <f ca="1">RANDBETWEEN(1,9999999)</f>
-        <v>4445135</v>
+        <v>3128594</v>
       </c>
       <c r="C6">
         <f ca="1">B6</f>
-        <v>4445135</v>
+        <v>3128594</v>
       </c>
     </row>
   </sheetData>
@@ -606,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C88DEB-9E29-46A7-A0A0-738E5711FB06}">
   <dimension ref="A6:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>